<commit_message>
correcciones de missing values
</commit_message>
<xml_diff>
--- a/Datos prueba.xlsx
+++ b/Datos prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Juli\Abejorros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EABE223-4A02-44F1-A257-7214AB812BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29794D18-14FA-42D1-BC40-284B239D3568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="10240" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Limpio" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4614" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4612" uniqueCount="164">
   <si>
     <t>PER 24hs</t>
   </si>
@@ -3705,10 +3705,10 @@
   </sheetPr>
   <dimension ref="A1:AE999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="D138" sqref="D138"/>
+      <selection pane="bottomLeft" activeCell="W212" sqref="W212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4222,7 +4222,9 @@
       <c r="T7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U7" s="1"/>
+      <c r="U7" s="1">
+        <v>1</v>
+      </c>
       <c r="V7" s="1" t="s">
         <v>27</v>
       </c>
@@ -4295,6 +4297,9 @@
         <v>0</v>
       </c>
       <c r="U8" s="1">
+        <v>0</v>
+      </c>
+      <c r="V8" s="95">
         <v>0</v>
       </c>
       <c r="W8" s="1">
@@ -4608,8 +4613,8 @@
       <c r="V12" s="1">
         <v>0</v>
       </c>
-      <c r="W12" s="1" t="s">
-        <v>27</v>
+      <c r="W12" s="1">
+        <v>0</v>
       </c>
       <c r="X12" s="1">
         <v>2.8999999999999915E-2</v>
@@ -4676,7 +4681,9 @@
       <c r="T13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U13" s="1"/>
+      <c r="U13" s="1">
+        <v>1</v>
+      </c>
       <c r="V13" s="1" t="s">
         <v>29</v>
       </c>
@@ -4755,8 +4762,8 @@
       <c r="V14" s="1">
         <v>0</v>
       </c>
-      <c r="W14" s="1" t="s">
-        <v>27</v>
+      <c r="W14" s="1">
+        <v>0</v>
       </c>
       <c r="X14" s="1">
         <v>0.17600000000000016</v>
@@ -4829,7 +4836,9 @@
       <c r="T15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U15" s="1"/>
+      <c r="U15" s="1">
+        <v>1</v>
+      </c>
       <c r="V15" s="1" t="s">
         <v>29</v>
       </c>
@@ -5581,8 +5590,12 @@
       <c r="T25" s="1">
         <v>0</v>
       </c>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
+      <c r="U25" s="1">
+        <v>1</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="W25" s="1" t="s">
         <v>29</v>
       </c>
@@ -5652,8 +5665,12 @@
       <c r="T26" s="1">
         <v>0</v>
       </c>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
+      <c r="U26" s="1">
+        <v>1</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="W26" s="1" t="s">
         <v>29</v>
       </c>
@@ -5808,8 +5825,12 @@
       <c r="T28" s="1">
         <v>0</v>
       </c>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
+      <c r="U28" s="1">
+        <v>1</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="W28" s="1" t="s">
         <v>29</v>
       </c>
@@ -5882,7 +5903,9 @@
       <c r="U29" s="1">
         <v>1</v>
       </c>
-      <c r="V29" s="1"/>
+      <c r="V29" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="W29" s="1" t="s">
         <v>29</v>
       </c>
@@ -6492,10 +6515,10 @@
         <v>1</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="X37" s="1">
         <v>0.1628</v>
@@ -8388,9 +8411,11 @@
       <c r="U63" s="1">
         <v>1</v>
       </c>
-      <c r="V63" s="1"/>
-      <c r="W63" s="1" t="s">
-        <v>27</v>
+      <c r="V63" s="1">
+        <v>0</v>
+      </c>
+      <c r="W63" s="1">
+        <v>0</v>
       </c>
       <c r="X63" s="1">
         <v>0.26929999999999998</v>
@@ -8763,9 +8788,11 @@
       <c r="U68" s="1">
         <v>1</v>
       </c>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1" t="s">
-        <v>27</v>
+      <c r="V68" s="1">
+        <v>0</v>
+      </c>
+      <c r="W68" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:31" ht="12.5" x14ac:dyDescent="0.25">
@@ -8832,9 +8859,11 @@
       <c r="U69" s="1">
         <v>1</v>
       </c>
-      <c r="V69" s="1"/>
-      <c r="W69" s="1" t="s">
-        <v>27</v>
+      <c r="V69" s="1">
+        <v>0</v>
+      </c>
+      <c r="W69" s="1">
+        <v>0</v>
       </c>
       <c r="Y69" s="2"/>
       <c r="Z69" s="2"/>
@@ -9058,11 +9087,11 @@
       <c r="U72" s="1">
         <v>1</v>
       </c>
-      <c r="V72" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W72" s="1" t="s">
-        <v>27</v>
+      <c r="V72" s="1">
+        <v>0</v>
+      </c>
+      <c r="W72" s="1">
+        <v>0</v>
       </c>
       <c r="Y72" s="2"/>
       <c r="Z72" s="2"/>
@@ -9367,11 +9396,11 @@
       <c r="U76" s="1">
         <v>1</v>
       </c>
-      <c r="V76" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W76" s="1" t="s">
-        <v>27</v>
+      <c r="V76" s="1">
+        <v>0</v>
+      </c>
+      <c r="W76" s="1">
+        <v>0</v>
       </c>
       <c r="X76" s="1">
         <v>0.1391</v>
@@ -9441,11 +9470,11 @@
       <c r="U77" s="1">
         <v>1</v>
       </c>
-      <c r="V77" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W77" s="1" t="s">
-        <v>27</v>
+      <c r="V77" s="1">
+        <v>0</v>
+      </c>
+      <c r="W77" s="1">
+        <v>0</v>
       </c>
       <c r="X77" s="1">
         <v>0.1235</v>
@@ -9660,11 +9689,11 @@
       <c r="U80" s="1">
         <v>0</v>
       </c>
-      <c r="V80" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W80" s="1" t="s">
-        <v>27</v>
+      <c r="V80" s="1">
+        <v>0</v>
+      </c>
+      <c r="W80" s="1">
+        <v>0</v>
       </c>
       <c r="X80" s="1">
         <v>0.24900000000000055</v>
@@ -9962,9 +9991,11 @@
       <c r="U84" s="1">
         <v>0</v>
       </c>
-      <c r="V84" s="1"/>
-      <c r="W84" s="1" t="s">
-        <v>27</v>
+      <c r="V84" s="1">
+        <v>0</v>
+      </c>
+      <c r="W84" s="1">
+        <v>0</v>
       </c>
       <c r="X84" s="1">
         <v>0.28900000000000148</v>
@@ -10633,9 +10664,11 @@
       <c r="U93" s="1">
         <v>1</v>
       </c>
-      <c r="V93" s="1"/>
+      <c r="V93" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="W93" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="X93" s="101">
         <v>0.2068999999999992</v>
@@ -11610,10 +11643,10 @@
         <v>1</v>
       </c>
       <c r="V106" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="W106" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="X106" s="1">
         <v>0.16219999999999857</v>
@@ -15643,10 +15676,10 @@
         <v>1</v>
       </c>
       <c r="V160" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="W160" s="106">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="W160" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="X160" s="106">
         <v>-0.20119999999999999</v>
@@ -16314,9 +16347,11 @@
       <c r="U169" s="92">
         <v>1</v>
       </c>
-      <c r="V169" s="106"/>
-      <c r="W169" s="106">
-        <v>0</v>
+      <c r="V169" s="106" t="s">
+        <v>29</v>
+      </c>
+      <c r="W169" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="X169" s="106">
         <v>0.27600000000000002</v>
@@ -16386,9 +16421,11 @@
       <c r="U170" s="92">
         <v>1</v>
       </c>
-      <c r="V170" s="106"/>
-      <c r="W170" s="106">
-        <v>0</v>
+      <c r="V170" s="106" t="s">
+        <v>29</v>
+      </c>
+      <c r="W170" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="X170" s="106">
         <v>0.1421</v>
@@ -18109,10 +18146,10 @@
         <v>1</v>
       </c>
       <c r="V195" s="124" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="W195" s="124" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="X195" s="123">
         <v>0.1452</v>
@@ -19128,8 +19165,12 @@
       <c r="U210" s="105">
         <v>1</v>
       </c>
-      <c r="V210" s="124"/>
-      <c r="W210" s="124"/>
+      <c r="V210" s="124" t="s">
+        <v>29</v>
+      </c>
+      <c r="W210" s="124" t="s">
+        <v>29</v>
+      </c>
       <c r="X210" s="123">
         <v>0.1593</v>
       </c>

</xml_diff>